<commit_message>
ADD test cases for borycheva
</commit_message>
<xml_diff>
--- a/Template_test_cases_borycheva.xlsx
+++ b/Template_test_cases_borycheva.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="312" windowWidth="15132" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="15135" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="21" r:id="rId1"/>
@@ -22,12 +22,12 @@
     <definedName name="Citing_Articles">'[3]General Search'!$B$9:$B$14</definedName>
     <definedName name="Results">'[4]General Search'!$B$9:$B$14</definedName>
   </definedNames>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <r>
       <t>How the tree directory is structured in Quality Center</t>
@@ -200,11 +200,132 @@
   <si>
     <t>INCI-2102</t>
   </si>
+  <si>
+    <t>Test cases for notebook</t>
+  </si>
+  <si>
+    <t>Notebook is launched. A new document was opened</t>
+  </si>
+  <si>
+    <t>Verify all item menu</t>
+  </si>
+  <si>
+    <t>Click the button File</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+all buttons are active: New, Open, Save, Save as, Page Setup, Print, Exit</t>
+  </si>
+  <si>
+    <t>Creat new file</t>
+  </si>
+  <si>
+    <t>Select an item New and click the button</t>
+  </si>
+  <si>
+    <t>create a new file</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Verifying the creation of a new file when the document is not full</t>
+  </si>
+  <si>
+    <t>Verifying the creation of a new file when the document is full</t>
+  </si>
+  <si>
+    <t>a dialog box opens</t>
+  </si>
+  <si>
+    <t>Click the button Save</t>
+  </si>
+  <si>
+    <t>Open new document</t>
+  </si>
+  <si>
+    <t>document saved</t>
+  </si>
+  <si>
+    <t>verification of the possibility of opening documents</t>
+  </si>
+  <si>
+    <t>Select an item Open and click the button</t>
+  </si>
+  <si>
+    <t>open the explorer window</t>
+  </si>
+  <si>
+    <t>Save new document</t>
+  </si>
+  <si>
+    <t>check the function of saving documents</t>
+  </si>
+  <si>
+    <t>write in document and click the button File</t>
+  </si>
+  <si>
+    <t>'hello world'</t>
+  </si>
+  <si>
+    <t>Select item Save</t>
+  </si>
+  <si>
+    <t>verification saving an existing document</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Save as</t>
+  </si>
+  <si>
+    <t>Page setup</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open new window with parameters </t>
+  </si>
+  <si>
+    <t>checking the options for setting page parameters</t>
+  </si>
+  <si>
+    <t>Select item Page setup and click the dutton</t>
+  </si>
+  <si>
+    <t>Print</t>
+  </si>
+  <si>
+    <t>verify printer choice for printing</t>
+  </si>
+  <si>
+    <t>Select item Print</t>
+  </si>
+  <si>
+    <t>pop-up window with settings print</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>verification to exit from program</t>
+  </si>
+  <si>
+    <t>Click the button Exit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end to work the program and close window </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -272,7 +393,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -293,6 +414,800 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -314,7 +1229,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -384,21 +1299,379 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -413,7 +1686,381 @@
     <cellStyle name="Normal_webofscience checklist" xfId="9"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="84">
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color indexed="13"/>
@@ -768,7 +2415,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -842,7 +2489,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -916,7 +2563,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -966,7 +2613,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -1090,6 +2737,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1124,6 +2772,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1299,133 +2948,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="106.6640625" customWidth="1"/>
+    <col min="1" max="1" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="25"/>
+      <c r="A2" s="24"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="25"/>
+      <c r="A3" s="24"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="25"/>
+      <c r="A6" s="24"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="24"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="24"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="24"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="24"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="24"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="24"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="24"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="25"/>
+      <c r="A21" s="24"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="25"/>
+      <c r="A22" s="24"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="25"/>
+      <c r="A23" s="24"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="25"/>
+      <c r="A24" s="24"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="25"/>
+      <c r="A25" s="24"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="25"/>
+      <c r="A26" s="24"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="25"/>
+      <c r="A27" s="24"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="25"/>
+      <c r="A28" s="24"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="25"/>
+      <c r="A29" s="24"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="25"/>
+      <c r="A30" s="24"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="25"/>
+      <c r="A32" s="24"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="25"/>
+      <c r="A33" s="24"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="25"/>
+      <c r="A34" s="24"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="25"/>
+      <c r="A35" s="24"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="25"/>
+      <c r="A36" s="24"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="25"/>
+      <c r="A37" s="24"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="25"/>
+      <c r="A38" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1438,28 +3087,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="10"/>
-    <col min="3" max="3" width="9.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="33.44140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="11"/>
-    <col min="7" max="7" width="62" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="63.5546875" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="10"/>
+    <col min="1" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="9.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
+    <col min="7" max="7" width="54.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="63.5703125" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" ht="66">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="63.75">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +3167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="52.8">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="51">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1537,7 +3186,7 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="4"/>
@@ -1555,7 +3204,7 @@
       <c r="R2" s="9"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:19" s="12" customFormat="1">
+    <row r="3" spans="1:19" s="12" customFormat="1" ht="25.5">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
@@ -1582,10 +3231,10 @@
       <c r="R3" s="9"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="26.4">
+    <row r="4" spans="1:19" s="12" customFormat="1" ht="25.5">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="23"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3">
@@ -1612,16 +3261,18 @@
       <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19" s="12" customFormat="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="13"/>
+      <c r="A5" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
@@ -1632,17 +3283,33 @@
       <c r="R5" s="16"/>
       <c r="S5" s="14"/>
     </row>
-    <row r="6" spans="1:19" s="12" customFormat="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="13"/>
+    <row r="6" spans="1:19" s="12" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A6" s="33">
+        <v>1</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="36">
+        <v>1</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="28"/>
+      <c r="I6" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="30"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
@@ -1653,17 +3320,31 @@
       <c r="R6" s="16"/>
       <c r="S6" s="14"/>
     </row>
-    <row r="7" spans="1:19" s="12" customFormat="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="13"/>
+    <row r="7" spans="1:19" s="12" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A7" s="47">
+        <v>2</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="44">
+        <v>1</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="37"/>
+      <c r="I7" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="38"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
@@ -1675,16 +3356,20 @@
       <c r="S7" s="14"/>
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="13"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="43">
+        <v>2</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="38"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -1695,16 +3380,32 @@
       <c r="R8" s="16"/>
       <c r="S8" s="14"/>
     </row>
-    <row r="9" spans="1:19" s="12" customFormat="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+    <row r="9" spans="1:19" s="12" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A9" s="68">
+        <v>3</v>
+      </c>
+      <c r="B9" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="73">
+        <v>1</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="76" t="s">
+        <v>44</v>
+      </c>
       <c r="J9" s="13"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
@@ -1720,12 +3421,16 @@
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="73">
+        <v>2</v>
+      </c>
+      <c r="G10" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="74"/>
+      <c r="I10" s="77"/>
       <c r="J10" s="13"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
@@ -1738,15 +3443,21 @@
       <c r="S10" s="14"/>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A11" s="17"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="75">
+        <v>3</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="78" t="s">
+        <v>47</v>
+      </c>
       <c r="J11" s="13"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
@@ -1758,16 +3469,30 @@
       <c r="R11" s="16"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:19" s="12" customFormat="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="19"/>
+    <row r="12" spans="1:19" s="12" customFormat="1" ht="38.25">
+      <c r="A12" s="64">
+        <v>4</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="56">
+        <v>1</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="53"/>
+      <c r="I12" s="54" t="s">
+        <v>50</v>
+      </c>
       <c r="J12" s="13"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -1779,16 +3504,17 @@
       <c r="R12" s="16"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:19" s="12" customFormat="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="19"/>
+    <row r="13" spans="1:19" s="12" customFormat="1" ht="25.5" customHeight="1">
+      <c r="D13" s="91"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="56">
+        <v>2</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="13"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -1800,224 +3526,597 @@
       <c r="R13" s="16"/>
       <c r="S13" s="14"/>
     </row>
+    <row r="14" spans="1:19" ht="40.5" customHeight="1">
+      <c r="A14" s="61">
+        <v>5</v>
+      </c>
+      <c r="B14" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="57">
+        <v>1</v>
+      </c>
+      <c r="G14" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="D15" s="25"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="82">
+        <v>2</v>
+      </c>
+      <c r="G15" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="81"/>
+      <c r="I15" s="84"/>
+    </row>
+    <row r="16" spans="1:19" ht="25.5" customHeight="1">
+      <c r="A16" s="89">
+        <v>6</v>
+      </c>
+      <c r="B16" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="92" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="86">
+        <v>1</v>
+      </c>
+      <c r="G16" s="87" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="83"/>
+      <c r="I16" s="85" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="100"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="107">
+        <v>2</v>
+      </c>
+      <c r="G17" s="108" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="83"/>
+      <c r="I17" s="112"/>
+    </row>
+    <row r="18" spans="1:9" ht="32.25" customHeight="1">
+      <c r="A18" s="103">
+        <v>7</v>
+      </c>
+      <c r="B18" s="104" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="105" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="109" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="110">
+        <v>1</v>
+      </c>
+      <c r="G18" s="111" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="114"/>
+      <c r="I18" s="113" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="115"/>
+      <c r="C19" s="116"/>
+      <c r="E19" s="115"/>
+      <c r="G19" s="111" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="114"/>
+      <c r="I19" s="120"/>
+    </row>
+    <row r="20" spans="1:9" ht="25.5">
+      <c r="A20" s="117">
+        <v>8</v>
+      </c>
+      <c r="B20" s="118" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="121" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="124">
+        <v>1</v>
+      </c>
+      <c r="G20" s="123" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="118"/>
+      <c r="I20" s="122" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A21" s="125"/>
+      <c r="C21" s="126"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="134">
+        <v>2</v>
+      </c>
+      <c r="G21" s="118" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="118"/>
+      <c r="I21" s="135"/>
+    </row>
+    <row r="22" spans="1:9" ht="31.5" customHeight="1">
+      <c r="A22" s="127">
+        <v>9</v>
+      </c>
+      <c r="B22" s="128" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="129" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="136" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="137">
+        <v>1</v>
+      </c>
+      <c r="G22" s="128" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="128"/>
+      <c r="I22" s="138" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A23" s="130"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="140">
+        <v>2</v>
+      </c>
+      <c r="G23" s="131" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="131"/>
+      <c r="I23" s="141"/>
+    </row>
+    <row r="24" spans="1:9" ht="25.5">
+      <c r="A24" s="80">
+        <v>10</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="11">
+        <v>1</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="F25" s="11">
+        <v>2</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I4 G4:G6 I12:I13 G12:G13">
-    <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="80" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="81" stopIfTrue="1" operator="equal">
+  <mergeCells count="21">
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="E9:E11"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I4 G4 I12 G12:G13 G6:G7">
+    <cfRule type="cellIs" priority="127" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="128" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="129" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 G4:G6 I12:I13 G12:G13">
-    <cfRule type="cellIs" priority="76" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="77" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="78" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="I4 G4 I12 G12:G13 G6:G7">
+    <cfRule type="cellIs" priority="124" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="125" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="126" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3 G3:G4">
-    <cfRule type="cellIs" priority="58" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="59" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="106" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="107" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="108" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3 G3:G4">
-    <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="56" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="103" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="104" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="105" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3">
-    <cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="53" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="100" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="101" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="102" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3">
-    <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="50" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="97" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="98" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="99" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" priority="46" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="47" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="94" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="95" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="96" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="44" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="45" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="41" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="42" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="38" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="39" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="35" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="36" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="32" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="91" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="92" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="93" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="29" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="76" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="77" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="78" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="26" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="73" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="74" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="75" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="23" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="70" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="71" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="72" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="20" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="68" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="69" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="64" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="65" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="66" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
+    <cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="62" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="63" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:I7 G8:H8 H9:I9 G11:I11 G10:H10">
+    <cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="53" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="54" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:I7 G8:H8 H9:I9 G11:I11 G10:H10">
+    <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="50" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="51" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" priority="46" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="47" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="48" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="44" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="45" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="41" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="42" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="38" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="39" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="35" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="36" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="32" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="33" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="29" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="30" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="26" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="27" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="23" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="24" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="21" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="17" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="18" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I11">
+  <conditionalFormatting sqref="G19">
+    <cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
     <cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I11">
+  <conditionalFormatting sqref="I18">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
UPD checked test cases
</commit_message>
<xml_diff>
--- a/Template_test_cases_borycheva.xlsx
+++ b/Template_test_cases_borycheva.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekaterina.andronova\Downloads\skillup1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="312" windowWidth="15132" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="15135" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="21" r:id="rId1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
   <si>
     <r>
       <t>How the tree directory is structured in Quality Center</t>
@@ -308,12 +313,42 @@
   <si>
     <t xml:space="preserve">Click 'save' </t>
   </si>
+  <si>
+    <t>Prerequisites должен быть в нашем случае для каждого кейса</t>
+  </si>
+  <si>
+    <t>Лучше в пассиве написать, что context menu is opened…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Описать что именно происходит в Expected </t>
+  </si>
+  <si>
+    <t>Какой именно dialog window? Что оно спрашивает. Описать</t>
+  </si>
+  <si>
+    <t>Проверить что правда сохранилось</t>
+  </si>
+  <si>
+    <t>Этот кейс можно обьединить с предыдущим</t>
+  </si>
+  <si>
+    <t>Prerequisites должен быть в нашем случае для каждого кейса, Лучше в пассиве написать, что context menu is opened…</t>
+  </si>
+  <si>
+    <t>расписать, нам же надо проверить что документ откроется, а не explorer window</t>
+  </si>
+  <si>
+    <t>расписать проверку что при изменении параметров они правда меняют что-то на странице</t>
+  </si>
+  <si>
+    <t>Расписать закрытие пустого файла, с текстом сохраненного, с текстом не сохраненного</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +402,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -464,7 +514,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -489,10 +539,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -517,12 +563,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -585,98 +625,112 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Hyperlink 3" xfId="1"/>
     <cellStyle name="Hyperlink 4" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 18" xfId="3"/>
     <cellStyle name="Normal 4 3" xfId="4"/>
     <cellStyle name="Normal 8 3" xfId="5"/>
@@ -684,43 +738,8 @@
     <cellStyle name="Normal 8 5" xfId="7"/>
     <cellStyle name="Normal 8 6" xfId="8"/>
     <cellStyle name="Normal_webofscience checklist" xfId="9"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <color indexed="13"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color indexed="13"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="51"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <font>
         <color indexed="13"/>
@@ -1357,9 +1376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1397,9 +1416,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1434,7 +1453,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1469,7 +1488,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1649,126 +1668,126 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="106.6640625" customWidth="1"/>
+    <col min="1" max="1" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="16"/>
+      <c r="A2" s="52"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="16"/>
+      <c r="A3" s="52"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="16"/>
+      <c r="A4" s="52"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="16"/>
+      <c r="A5" s="52"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="16"/>
+      <c r="A6" s="52"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="16"/>
+      <c r="A7" s="52"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="16"/>
+      <c r="A8" s="52"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="16"/>
+      <c r="A9" s="52"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="16"/>
+      <c r="A10" s="52"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="16"/>
+      <c r="A11" s="52"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="16"/>
+      <c r="A12" s="52"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="16"/>
+      <c r="A13" s="52"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="16"/>
+      <c r="A14" s="52"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="16"/>
+      <c r="A15" s="52"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="16"/>
+      <c r="A16" s="52"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="16"/>
+      <c r="A17" s="52"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="16"/>
+      <c r="A18" s="52"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="16"/>
+      <c r="A19" s="52"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="16"/>
+      <c r="A20" s="52"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="16"/>
+      <c r="A21" s="52"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="16"/>
+      <c r="A22" s="52"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="16"/>
+      <c r="A23" s="52"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="16"/>
+      <c r="A24" s="52"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="16"/>
+      <c r="A25" s="52"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="16"/>
+      <c r="A26" s="52"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="16"/>
+      <c r="A27" s="52"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="16"/>
+      <c r="A28" s="52"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="16"/>
+      <c r="A29" s="52"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="16"/>
+      <c r="A30" s="52"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="16"/>
+      <c r="A31" s="52"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="16"/>
+      <c r="A32" s="52"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="16"/>
+      <c r="A33" s="52"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="16"/>
+      <c r="A34" s="52"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="16"/>
+      <c r="A35" s="52"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="16"/>
+      <c r="A36" s="52"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="16"/>
+      <c r="A37" s="52"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="16"/>
+      <c r="A38" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1786,51 +1805,52 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="4"/>
-    <col min="3" max="3" width="9.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="5"/>
-    <col min="7" max="7" width="54.109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="63.5546875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="9.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="54.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="63.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="52.85546875" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" ht="66">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:19" s="6" customFormat="1" ht="63.75">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -1862,340 +1882,357 @@
       </c>
     </row>
     <row r="2" spans="1:19" s="6" customFormat="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="8"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A3" s="23">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="25">
         <v>1</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="25" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="8"/>
+      <c r="J3" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="42">
+      <c r="A4" s="54">
         <v>2</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="35">
         <v>1</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="8"/>
-    </row>
-    <row r="5" spans="1:19" s="6" customFormat="1" ht="13.8" thickBot="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28">
+      <c r="J4" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" spans="1:19" s="6" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25">
         <v>2</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="31" t="s">
+      <c r="H5" s="22"/>
+      <c r="I5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="8"/>
+      <c r="J5" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A6" s="48">
+      <c r="A6" s="38">
         <v>3</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38" t="s">
+      <c r="D6" s="33"/>
+      <c r="E6" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="35">
         <v>1</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="I6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="8"/>
-    </row>
-    <row r="7" spans="1:19" s="6" customFormat="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22">
+      <c r="J6" s="62"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" s="6" customFormat="1" ht="25.5">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19">
         <v>2</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="30" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="8"/>
+      <c r="J7" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" s="6" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25">
         <v>3</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="8"/>
+      <c r="J8" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="42" customHeight="1" thickBot="1">
-      <c r="A9" s="51">
+      <c r="A9" s="41">
         <v>4</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="46">
         <v>1</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53" t="s">
+      <c r="H9" s="43"/>
+      <c r="I9" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="8"/>
-    </row>
-    <row r="10" spans="1:19" s="6" customFormat="1" ht="26.4">
-      <c r="A10" s="48">
+      <c r="J9" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" spans="1:19" s="6" customFormat="1" ht="38.25">
+      <c r="A10" s="38">
         <v>5</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="44" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="35">
         <v>1</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="41" t="s">
+      <c r="H10" s="34"/>
+      <c r="I10" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="8"/>
+      <c r="J10" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="28">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="25">
         <v>2</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="27"/>
-      <c r="I11" s="31" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="8"/>
+      <c r="J11" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="40.5" customHeight="1">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="21" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="16" t="s">
         <v>59</v>
       </c>
+      <c r="J12" s="63"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="D13" s="18"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="5">
         <v>2</v>
       </c>
@@ -2205,26 +2242,30 @@
       <c r="I13" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="13.8" thickBot="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="57">
+      <c r="J13" s="63"/>
+    </row>
+    <row r="14" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="47">
         <v>3</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29" t="s">
+      <c r="H14" s="26"/>
+      <c r="I14" s="26" t="s">
         <v>32</v>
       </c>
+      <c r="J14" s="62" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2233,39 +2274,43 @@
       <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="5">
         <v>1</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" ht="13.8" thickBot="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="57">
+      <c r="J15" s="63"/>
+    </row>
+    <row r="16" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="47">
         <v>2</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29" t="s">
+      <c r="H16" s="26"/>
+      <c r="I16" s="26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="32.25" customHeight="1">
-      <c r="A17" s="14">
+      <c r="J16" s="62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="32.25" customHeight="1">
+      <c r="A17" s="13">
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2274,121 +2319,131 @@
       <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F17" s="5">
         <v>1</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="13.8" thickBot="1">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="25" t="s">
+      <c r="J17" s="63"/>
+    </row>
+    <row r="18" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="31" t="s">
+      <c r="H18" s="26"/>
+      <c r="I18" s="28" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="26.4">
-      <c r="A19" s="58">
+      <c r="J18" s="62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="25.5">
+      <c r="A19" s="48">
         <v>9</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="32"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="61">
+      <c r="F19" s="50">
         <v>1</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="29"/>
+      <c r="I19" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="13.8" thickBot="1">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="57">
+      <c r="J19" s="63"/>
+    </row>
+    <row r="20" spans="1:10" ht="26.25" thickBot="1">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="47">
         <v>2</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29" t="s">
+      <c r="H20" s="26"/>
+      <c r="I20" s="26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="31.5" customHeight="1">
-      <c r="A21" s="58">
+      <c r="J20" s="63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="31.5" customHeight="1">
+      <c r="A21" s="48">
         <v>10</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="32"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="61">
+      <c r="F21" s="50">
         <v>1</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="19" t="s">
+      <c r="H21" s="29"/>
+      <c r="I21" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="13.8" thickBot="1">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="57">
+      <c r="J21" s="63"/>
+    </row>
+    <row r="22" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="47">
         <v>2</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29" t="s">
+      <c r="H22" s="26"/>
+      <c r="I22" s="26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="26.4">
-      <c r="A23" s="14">
+      <c r="J22" s="63"/>
+    </row>
+    <row r="23" spans="1:10" ht="25.5">
+      <c r="A23" s="13">
         <v>11</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2406,11 +2461,14 @@
       <c r="G23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="63" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="F24" s="5">
         <v>2</v>
       </c>
@@ -2423,22 +2481,22 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E21:E22"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E21:E22"/>
   </mergeCells>
   <conditionalFormatting sqref="I11 G10:G11 G3:G4">
     <cfRule type="cellIs" priority="133" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="134" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="135" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="134" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="135" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2446,10 +2504,10 @@
     <cfRule type="cellIs" priority="130" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="131" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="132" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="131" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="132" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2457,10 +2515,10 @@
     <cfRule type="cellIs" priority="70" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="71" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="71" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="72" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2468,10 +2526,10 @@
     <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="68" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="68" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="69" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2479,10 +2537,10 @@
     <cfRule type="cellIs" priority="58" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="59" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="59" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="60" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2490,10 +2548,10 @@
     <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="56" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="56" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="57" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2501,10 +2559,10 @@
     <cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="53" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="53" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="54" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2512,10 +2570,10 @@
     <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="50" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="50" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="51" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2523,10 +2581,10 @@
     <cfRule type="cellIs" priority="46" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="47" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="47" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="48" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2534,10 +2592,10 @@
     <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="44" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="44" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="45" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2545,10 +2603,10 @@
     <cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="41" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="41" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="42" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2556,10 +2614,10 @@
     <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="38" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="38" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="39" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2567,10 +2625,10 @@
     <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="35" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="35" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="36" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2578,10 +2636,10 @@
     <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="32" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="32" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="33" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ADD test cases modified for borycheva
</commit_message>
<xml_diff>
--- a/Template_test_cases_borycheva.xlsx
+++ b/Template_test_cases_borycheva.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekaterina.andronova\Downloads\skillup1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="315" windowWidth="15135" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
   </bookViews>
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
   <si>
     <r>
       <t>How the tree directory is structured in Quality Center</t>
@@ -191,15 +186,9 @@
     <t>Select an item New and click the button</t>
   </si>
   <si>
-    <t>create a new file</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>a dialog box opens</t>
-  </si>
-  <si>
     <t>Click the button Save</t>
   </si>
   <si>
@@ -215,9 +204,6 @@
     <t>Select an item Open and click the button</t>
   </si>
   <si>
-    <t>open the explorer window</t>
-  </si>
-  <si>
     <t>Save new document</t>
   </si>
   <si>
@@ -269,9 +255,6 @@
     <t>Exit</t>
   </si>
   <si>
-    <t>verification to exit from program</t>
-  </si>
-  <si>
     <t>Click the button Exit</t>
   </si>
   <si>
@@ -284,12 +267,6 @@
     <t>Verifying the creation of a new file when the document is not empty</t>
   </si>
   <si>
-    <t>open context menu with functions: New, Open, Save, Save as, Page Setup, Print, Exit (all active items)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open context menu </t>
-  </si>
-  <si>
     <t>type text in document and click the button File</t>
   </si>
   <si>
@@ -299,9 +276,6 @@
     <t>Create</t>
   </si>
   <si>
-    <t>check the saving of the document in the directory</t>
-  </si>
-  <si>
     <t>Open default directory</t>
   </si>
   <si>
@@ -314,41 +288,65 @@
     <t xml:space="preserve">Click 'save' </t>
   </si>
   <si>
-    <t>Prerequisites должен быть в нашем случае для каждого кейса</t>
-  </si>
-  <si>
-    <t>Лучше в пассиве написать, что context menu is opened…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Описать что именно происходит в Expected </t>
-  </si>
-  <si>
-    <t>Какой именно dialog window? Что оно спрашивает. Описать</t>
-  </si>
-  <si>
-    <t>Проверить что правда сохранилось</t>
-  </si>
-  <si>
-    <t>Этот кейс можно обьединить с предыдущим</t>
-  </si>
-  <si>
-    <t>Prerequisites должен быть в нашем случае для каждого кейса, Лучше в пассиве написать, что context menu is opened…</t>
-  </si>
-  <si>
-    <t>расписать, нам же надо проверить что документ откроется, а не explorer window</t>
-  </si>
-  <si>
-    <t>расписать проверку что при изменении параметров они правда меняют что-то на странице</t>
-  </si>
-  <si>
-    <t>Расписать закрытие пустого файла, с текстом сохраненного, с текстом не сохраненного</t>
+    <t>context menu is opened with functions: New, Open, Save, Save as, Page Setup, Print, Exit (all active items)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> context menu  is opened</t>
+  </si>
+  <si>
+    <t>a new blank notepad was displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialog window  is displayed "save or not" </t>
+  </si>
+  <si>
+    <t>the explorer window with the documents for selection is opened.</t>
+  </si>
+  <si>
+    <t>123.txt</t>
+  </si>
+  <si>
+    <t>Select document and click Open button</t>
+  </si>
+  <si>
+    <t>the file was displayed</t>
+  </si>
+  <si>
+    <t>the explorer window for selection is opened.</t>
+  </si>
+  <si>
+    <t>the default folder displays the saved document</t>
+  </si>
+  <si>
+    <t>changes was displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сhange some page parameters and Click "OK" </t>
+  </si>
+  <si>
+    <t>verification to exit from program when  the document is not empty</t>
+  </si>
+  <si>
+    <t>verification to exit from program when  the document is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Not save" </t>
+  </si>
+  <si>
+    <t>notepad is close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verification to exit from program when  the document  saved </t>
+  </si>
+  <si>
+    <t>Notebook is launched. A document was opened</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +419,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="6"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -430,7 +436,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -484,17 +490,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -514,7 +509,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -625,9 +620,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -652,42 +644,49 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -713,24 +712,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Hyperlink 3" xfId="1"/>
     <cellStyle name="Hyperlink 4" xfId="2"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 18" xfId="3"/>
     <cellStyle name="Normal 4 3" xfId="4"/>
     <cellStyle name="Normal 8 3" xfId="5"/>
@@ -738,8 +736,349 @@
     <cellStyle name="Normal 8 5" xfId="7"/>
     <cellStyle name="Normal 8 6" xfId="8"/>
     <cellStyle name="Normal_webofscience checklist" xfId="9"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="84">
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="51"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color indexed="13"/>
@@ -1376,9 +1715,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1416,9 +1755,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1453,7 +1792,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1488,7 +1827,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1674,120 +2013,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="52"/>
+      <c r="A2" s="51"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="52"/>
+      <c r="A3" s="51"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="52"/>
+      <c r="A4" s="51"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="52"/>
+      <c r="A5" s="51"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="52"/>
+      <c r="A6" s="51"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="52"/>
+      <c r="A7" s="51"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="52"/>
+      <c r="A8" s="51"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="52"/>
+      <c r="A9" s="51"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="52"/>
+      <c r="A10" s="51"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="52"/>
+      <c r="A11" s="51"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="52"/>
+      <c r="A12" s="51"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="52"/>
+      <c r="A13" s="51"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="52"/>
+      <c r="A14" s="51"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="52"/>
+      <c r="A15" s="51"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="52"/>
+      <c r="A16" s="51"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="52"/>
+      <c r="A17" s="51"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="52"/>
+      <c r="A18" s="51"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="52"/>
+      <c r="A19" s="51"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="52"/>
+      <c r="A20" s="51"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="52"/>
+      <c r="A21" s="51"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="52"/>
+      <c r="A22" s="51"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="52"/>
+      <c r="A23" s="51"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="52"/>
+      <c r="A24" s="51"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="52"/>
+      <c r="A25" s="51"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="52"/>
+      <c r="A26" s="51"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="52"/>
+      <c r="A27" s="51"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="52"/>
+      <c r="A28" s="51"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="52"/>
+      <c r="A29" s="51"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="52"/>
+      <c r="A30" s="51"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="52"/>
+      <c r="A31" s="51"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="52"/>
+      <c r="A32" s="51"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="52"/>
+      <c r="A33" s="51"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="52"/>
+      <c r="A34" s="51"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="52"/>
+      <c r="A35" s="51"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="52"/>
+      <c r="A36" s="51"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="52"/>
+      <c r="A37" s="51"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="52"/>
+      <c r="A38" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1801,11 +2140,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1882,18 +2221,18 @@
       </c>
     </row>
     <row r="2" spans="1:19" s="6" customFormat="1">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -1914,7 +2253,7 @@
       <c r="C3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="22" t="s">
@@ -1928,11 +2267,9 @@
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="62" t="s">
-        <v>69</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="J3" s="61"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1944,32 +2281,32 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A4" s="54">
+      <c r="A4" s="55">
         <v>2</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="34">
+        <v>1</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="35">
-        <v>1</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="62" t="s">
-        <v>68</v>
-      </c>
+      <c r="J4" s="61"/>
       <c r="K4" s="11"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -1981,10 +2318,10 @@
       <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="24"/>
       <c r="F5" s="25">
         <v>2</v>
@@ -1994,11 +2331,9 @@
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="62" t="s">
-        <v>70</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="J5" s="61"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -2010,32 +2345,34 @@
       <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A6" s="38">
+      <c r="A6" s="37">
         <v>3</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="35">
+      <c r="B6" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="34">
         <v>1</v>
       </c>
-      <c r="G6" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="62"/>
+      <c r="G6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="48"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -2046,7 +2383,7 @@
       <c r="R6" s="9"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:19" s="6" customFormat="1" ht="25.5">
+    <row r="7" spans="1:19" s="6" customFormat="1">
       <c r="A7" s="10"/>
       <c r="B7" s="12"/>
       <c r="C7" s="11"/>
@@ -2060,11 +2397,9 @@
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="62" t="s">
-        <v>71</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="J7" s="61"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -2075,25 +2410,22 @@
       <c r="R7" s="9"/>
       <c r="S7" s="7"/>
     </row>
-    <row r="8" spans="1:19" s="6" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25">
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B8" s="12"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19">
         <v>3</v>
       </c>
-      <c r="G8" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="62" t="s">
-        <v>72</v>
-      </c>
+      <c r="G8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="61"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -2105,30 +2437,22 @@
       <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="42" customHeight="1" thickBot="1">
-      <c r="A9" s="41">
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25">
         <v>4</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="46">
-        <v>1</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="62" t="s">
-        <v>73</v>
-      </c>
+      <c r="G9" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="61"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -2140,32 +2464,32 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" ht="38.25">
-      <c r="A10" s="38">
-        <v>5</v>
-      </c>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="37">
+        <v>4</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="35">
+      <c r="F10" s="34">
         <v>1</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="34"/>
-      <c r="I10" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="62" t="s">
-        <v>74</v>
-      </c>
+      <c r="H10" s="33"/>
+      <c r="I10" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="61"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -2176,25 +2500,20 @@
       <c r="R10" s="9"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="25">
+    <row r="11" spans="1:19" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="D11" s="15"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="19">
         <v>2</v>
       </c>
-      <c r="G11" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="62" t="s">
-        <v>75</v>
-      </c>
+      <c r="G11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="61"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -2205,121 +2524,121 @@
       <c r="R11" s="9"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:19" ht="40.5" customHeight="1">
-      <c r="A12" s="10">
+    <row r="12" spans="1:19" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="25">
+        <v>3</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="48"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" ht="40.5" customHeight="1">
+      <c r="A13" s="10">
+        <v>5</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="49"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="D14" s="15"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="5">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="49"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="D15" s="15"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="5">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="61"/>
+    </row>
+    <row r="16" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="40">
+        <v>4</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="48"/>
+    </row>
+    <row r="17" spans="1:10" ht="25.5" customHeight="1">
+      <c r="A17" s="13">
         <v>6</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="63"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="D13" s="15"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="5">
-        <v>2</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="63"/>
-    </row>
-    <row r="14" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="47">
-        <v>3</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A15" s="13">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J15" s="63"/>
-    </row>
-    <row r="16" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="47">
-        <v>2</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A17" s="13">
-        <v>8</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="4" t="s">
         <v>37</v>
       </c>
@@ -2330,404 +2649,691 @@
         <v>24</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="63"/>
-    </row>
-    <row r="18" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="49"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="D18" s="15"/>
+      <c r="F18" s="5">
+        <v>2</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="25.5">
-      <c r="A19" s="48">
-        <v>9</v>
-      </c>
-      <c r="B19" s="29" t="s">
+      <c r="J18" s="61"/>
+    </row>
+    <row r="19" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="40">
+        <v>3</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="48"/>
+    </row>
+    <row r="20" spans="1:10" ht="32.25" customHeight="1">
+      <c r="A20" s="13">
+        <v>7</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="61"/>
+    </row>
+    <row r="22" spans="1:10" ht="13.5" thickBot="1">
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" s="61"/>
+    </row>
+    <row r="23" spans="1:10" ht="38.25">
+      <c r="A23" s="41">
+        <v>8</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="50">
+      <c r="F23" s="43">
         <v>1</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G23" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" s="63"/>
-    </row>
-    <row r="20" spans="1:10" ht="26.25" thickBot="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="47">
-        <v>2</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="63" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="31.5" customHeight="1">
-      <c r="A21" s="48">
-        <v>10</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="50">
-        <v>1</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J21" s="63"/>
-    </row>
-    <row r="22" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="47">
-        <v>2</v>
-      </c>
-      <c r="G22" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="63"/>
-    </row>
-    <row r="23" spans="1:10" ht="25.5">
-      <c r="A23" s="13">
-        <v>11</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="H23" s="29"/>
       <c r="I23" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J23" s="63" t="s">
-        <v>77</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="J23" s="49"/>
     </row>
     <row r="24" spans="1:10">
+      <c r="A24" s="13"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="5">
         <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="J24" s="49"/>
+    </row>
+    <row r="25" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A25" s="13"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="5">
+        <v>3</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="49"/>
+    </row>
+    <row r="26" spans="1:10" ht="31.5" customHeight="1">
+      <c r="A26" s="41">
+        <v>9</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="43">
+        <v>1</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="29"/>
+      <c r="I26" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="49"/>
+    </row>
+    <row r="27" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="40">
+        <v>2</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="49"/>
+    </row>
+    <row r="28" spans="1:10" ht="38.25">
+      <c r="A28" s="13">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="49"/>
+    </row>
+    <row r="29" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="40">
+        <v>2</v>
+      </c>
+      <c r="G29" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="38.25">
+      <c r="A30" s="13">
+        <v>11</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="F31" s="5">
+        <v>2</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="40">
+        <v>3</v>
+      </c>
+      <c r="G32" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="38.25">
+      <c r="A33" s="13">
+        <v>12</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="F34" s="5">
+        <v>2</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E26:E27"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E10:E11"/>
   </mergeCells>
-  <conditionalFormatting sqref="I11 G10:G11 G3:G4">
-    <cfRule type="cellIs" priority="133" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="134" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="135" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="I11:I12 G10:G12 G3:G4">
+    <cfRule type="cellIs" priority="163" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="164" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="165" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11 G10:G11 G3:G4">
-    <cfRule type="cellIs" priority="130" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="131" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="132" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="I11:I12 G10:G12 G3:G4">
+    <cfRule type="cellIs" priority="160" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="161" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="162" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" priority="70" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="71" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="100" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="101" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="102" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3 H4 I5 H6 I7">
-    <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="68" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="97" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="98" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="99" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H5 G8:I9 G7:H7">
-    <cfRule type="cellIs" priority="58" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="59" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="88" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="89" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="90" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4 G5:I5 H6 G7:I9">
-    <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="56" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="85" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="86" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="87" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="53" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="82" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="83" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="84" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="80" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="81" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" priority="76" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="77" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="78" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" priority="73" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="74" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="75" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" priority="70" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="71" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="72" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="68" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="69" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" priority="64" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="65" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="66" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="62" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="63" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="53" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="54" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
     <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="50" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="50" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="51" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
+  <conditionalFormatting sqref="G21">
     <cfRule type="cellIs" priority="46" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="47" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="47" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="48" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
+  <conditionalFormatting sqref="G21">
     <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="44" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="44" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="45" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
+  <conditionalFormatting sqref="I21">
     <cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="41" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="41" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="42" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
+  <conditionalFormatting sqref="I21">
     <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="38" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="38" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="39" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="35" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="36" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="32" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="33" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="35" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="29" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="30" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="32" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="26" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="27" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
+  <conditionalFormatting sqref="I14">
     <cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="23" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="24" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
+  <conditionalFormatting sqref="I14">
     <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="20" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="20" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="21" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
+  <conditionalFormatting sqref="G19">
     <cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="17" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="18" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
+  <conditionalFormatting sqref="G19">
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="G22">
     <cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
+  <conditionalFormatting sqref="G22">
     <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
+  <conditionalFormatting sqref="I31">
     <cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
+  <conditionalFormatting sqref="I31">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>